<commit_message>
added RC filter values for stock pwm freq and increased pwm freq
</commit_message>
<xml_diff>
--- a/HIVE/motion/arduino/system_id/data/circuit_testing_data/RC_filter_test_data/RC_filt_vals.xlsx
+++ b/HIVE/motion/arduino/system_id/data/circuit_testing_data/RC_filter_test_data/RC_filt_vals.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\all my files\documents\uvm\5_masters\hive\github_directory\HIVE\motion\arduino\system_id\sys_id\RC_filter_test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\all my files\documents\uvm\5_masters\hive\github_directory\HIVE\motion\arduino\system_id\data\circuit_testing_data\RC_filter_test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0971A25A-9C9F-494C-8478-2E1D73442F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134FC859-49A3-4ED1-BBF0-A12F7D61994E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16410" windowWidth="29040" windowHeight="15840" xr2:uid="{18D000EC-40BF-43E8-ABF8-079CFB3258BD}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{18D000EC-40BF-43E8-ABF8-079CFB3258BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Fc [kHz]</t>
   </si>
@@ -56,6 +55,12 @@
   </si>
   <si>
     <t>v</t>
+  </si>
+  <si>
+    <t>for stock arduino pwm of 491 Hz, want cutoff freq around 1Hz</t>
+  </si>
+  <si>
+    <t>for sped up arduino pwm of 31372 Hz, try cutoff freq around 75 Hz</t>
   </si>
 </sst>
 </file>
@@ -108,6 +113,40 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{583C91C7-2F33-4D92-8095-1ED262661DFC}" name="Table1" displayName="Table1" ref="H1:K4" totalsRowShown="0">
+  <autoFilter ref="H1:K4" xr:uid="{583C91C7-2F33-4D92-8095-1ED262661DFC}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{DDB77220-4575-42BF-850D-EEE7A325810B}" name="C [nF]"/>
+    <tableColumn id="2" xr3:uid="{58690BDC-3BB5-44A0-B59F-53C86695CB56}" name="R [ohm]"/>
+    <tableColumn id="3" xr3:uid="{44C4FA88-DADC-42A6-B6A6-7C0857BA56B6}" name="Fc [Hz]">
+      <calculatedColumnFormula>1/(2*PI()*H2*10^-9*I2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{1A4F83C8-FE40-448E-AE50-B4B647494DAC}" name="Ts [ms]">
+      <calculatedColumnFormula>9.2*H2*10^-9*I2*1000</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{26D7C939-1428-4B5B-B160-6C086C3BC1EF}" name="Table3" displayName="Table3" ref="A1:D4" totalsRowShown="0">
+  <autoFilter ref="A1:D4" xr:uid="{26D7C939-1428-4B5B-B160-6C086C3BC1EF}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{30486F8A-9DCE-4EF6-8D64-F69B731E8F39}" name="Fc [kHz]"/>
+    <tableColumn id="2" xr3:uid="{C1A11E65-E499-4B6E-8814-209507ABB1A2}" name="C [nF]"/>
+    <tableColumn id="3" xr3:uid="{7D5234BF-5DA0-40BB-B0AB-E9B0DC36999B}" name="R [ohm]">
+      <calculatedColumnFormula>1/(2*PI()*A2*1000*B2*10^-9)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{9E780FBE-9C97-49A0-B30B-9B2B30770054}" name="Ts [ms]">
+      <calculatedColumnFormula>9.2*C2*B2*10^-9*1000</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -407,15 +446,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27D3D27-272D-4AD6-AD0A-2A41B91BD759}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -474,6 +518,66 @@
         <v>951.28</v>
       </c>
     </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1.5E-3</v>
+      </c>
+      <c r="B3">
+        <v>4700</v>
+      </c>
+      <c r="C3">
+        <f>1/(2*PI()*A3*1000*B3*10^-9)</f>
+        <v>22575.169232892953</v>
+      </c>
+      <c r="D3">
+        <f>9.2*C3*B3*10^-9*1000</f>
+        <v>976.15031763029128</v>
+      </c>
+      <c r="H3">
+        <v>4700</v>
+      </c>
+      <c r="I3">
+        <v>470</v>
+      </c>
+      <c r="J3">
+        <f>1/(2*PI()*H3*10^-9*I3)</f>
+        <v>72.048412445403045</v>
+      </c>
+      <c r="K3">
+        <f>9.2*H3*10^-9*I3*1000</f>
+        <v>20.322799999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.1</v>
+      </c>
+      <c r="B4">
+        <v>4700</v>
+      </c>
+      <c r="C4">
+        <f>1/(2*PI()*A4*1000*B4*10^-9)</f>
+        <v>338.6275384933943</v>
+      </c>
+      <c r="D4">
+        <f>9.2*C4*B4*10^-9*1000</f>
+        <v>14.642254764454368</v>
+      </c>
+      <c r="H4">
+        <v>47</v>
+      </c>
+      <c r="I4">
+        <v>47000</v>
+      </c>
+      <c r="J4">
+        <f>1/(2*PI()*H4*10^-9*I4)</f>
+        <v>72.048412445403045</v>
+      </c>
+      <c r="K4">
+        <f>9.2*H4*10^-9*I4*1000</f>
+        <v>20.322799999999997</v>
+      </c>
+    </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
@@ -491,7 +595,21 @@
         <v>2.2265625</v>
       </c>
     </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>